<commit_message>
presentation and xln done
</commit_message>
<xml_diff>
--- a/MPPiU/Маркетинг.xlsx
+++ b/MPPiU/Маркетинг.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baran\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labs\semester_5\MPPiU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68C396F-3EAE-44AE-8355-44F907FF2D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00244AF-DA03-4F43-899D-91D4EE555C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,128 +381,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -512,12 +395,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -526,9 +405,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -540,28 +416,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Нейтральный" xfId="2" builtinId="28"/>
@@ -948,7 +815,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1025,850 +892,850 @@
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
       <c r="H2">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>24</v>
       </c>
       <c r="H3">
         <v>4</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>24</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="1" t="s">
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>24</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="J5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="1" t="s">
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>24</v>
       </c>
       <c r="H6">
         <v>5</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6" s="1" t="s">
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s">
         <v>52</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
         <v>24</v>
       </c>
       <c r="H7">
         <v>4</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="1" t="s">
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" t="s">
         <v>28</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" t="s">
         <v>36</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>24</v>
       </c>
       <c r="H8">
         <v>5</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
         <v>41</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" s="1" t="s">
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" t="s">
         <v>28</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>24</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="J9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" s="1" t="s">
+      <c r="L9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" t="s">
         <v>59</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" t="s">
         <v>36</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s">
         <v>24</v>
       </c>
       <c r="H10">
         <v>5</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
         <v>62</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O10" s="1" t="s">
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" t="s">
         <v>63</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" t="s">
         <v>36</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" t="s">
         <v>66</v>
       </c>
       <c r="H11">
         <v>3</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
         <v>41</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" t="s">
         <v>34</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O11" s="1" t="s">
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" t="s">
         <v>67</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" t="s">
         <v>29</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" t="s">
         <v>24</v>
       </c>
       <c r="H12">
         <v>3</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="J12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
         <v>51</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" s="1" t="s">
+      <c r="M12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" t="s">
         <v>28</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" t="s">
         <v>29</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" t="s">
         <v>66</v>
       </c>
       <c r="H13">
         <v>5</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O13" s="1" t="s">
+      <c r="L13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" t="s">
         <v>73</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" t="s">
         <v>36</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
         <v>72</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" t="s">
         <v>24</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" t="s">
         <v>62</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L14" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N14" s="1" t="s">
+      <c r="M14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" t="s">
         <v>27</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="O14" t="s">
         <v>76</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="P14" t="s">
         <v>36</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" t="s">
         <v>24</v>
       </c>
       <c r="H15">
         <v>2</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" s="1" t="s">
+      <c r="L15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" t="s">
         <v>79</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="P15" t="s">
         <v>29</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="Q15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" t="s">
         <v>82</v>
       </c>
       <c r="H16">
         <v>4</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1" t="s">
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="1" t="s">
+      <c r="L16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" t="s">
         <v>34</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="N16" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="O16" t="s">
         <v>79</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="P16" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" t="s">
         <v>24</v>
       </c>
       <c r="H17">
         <v>3</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" t="s">
         <v>85</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" t="s">
         <v>51</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O17" s="1" t="s">
+      <c r="L17" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" t="s">
         <v>28</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="P17" t="s">
         <v>36</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="Q17" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1884,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1897,208 +1764,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>5</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
         <f>SUM(B2:D2)</f>
         <v>7</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
         <f>POWER(B2,2)/(B5*$E2)</f>
         <v>0.59523809523809523</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="3">
         <f>POWER(C2,2)/(C5*$E2)</f>
         <v>9.5238095238095233E-2</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="3">
         <f>POWER(D2,2)/(D5*$E2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
         <v>4</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <f t="shared" ref="E3:E4" si="0">SUM(B3:D3)</f>
         <v>4</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
         <f>POWER(B3,2)/(B$5*$E3)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <f t="shared" ref="H3:I4" si="1">POWER(C3,2)/(C$5*$E3)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
         <f>POWER(B4,2)/(B$5*$E4)</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <f t="shared" si="1"/>
         <v>0.53333333333333333</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <f>SUM(B2:B4)</f>
         <v>6</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <f t="shared" ref="C5:D5" si="2">SUM(C2:C4)</f>
         <v>6</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <f>SUM(G2:I4)-1</f>
         <v>1.2571428571428571</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="9">
-        <f>B8/((3-1)*(3-1))</f>
-        <v>0.31428571428571428</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="E8" s="6">
+        <f>SQRT(B8/((3-1)*(3-1)))</f>
+        <v>0.56061191058138804</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="10">
+      <c r="A12" s="7">
         <v>1</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="10">
+      <c r="A13" s="7">
         <v>2</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="5"/>
+      <c r="A14" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2114,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7233A6-401A-4C75-AF6E-F403650DF5B6}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2124,53 +1991,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="5">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="5">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
         <f>SUM(B2:F2)</f>
         <v>1</v>
       </c>
@@ -2182,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="J2:M6" si="0">POWER(D2,2)/(D$7*$G2)</f>
+        <f t="shared" ref="K2:L6" si="0">POWER(D2,2)/(D$7*$G2)</f>
         <v>0</v>
       </c>
       <c r="L2">
@@ -2194,25 +2061,25 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="5">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
         <f t="shared" ref="G3:G6" si="1">SUM(B3:F3)</f>
         <v>3</v>
       </c>
@@ -2236,25 +2103,25 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
         <v>3</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -2278,25 +2145,25 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -2320,25 +2187,25 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
         <v>3</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -2362,7 +2229,7 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B7">
@@ -2387,46 +2254,46 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B10">
         <f>SUM(I2:M6)-1</f>
         <v>0.52083333333333304</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="3">
-        <f>B10/((5-1)*(5-1))</f>
-        <v>3.2552083333333315E-2</v>
+      <c r="E10" s="1">
+        <f>SQRT(B10/((5-1)*(5-1)))</f>
+        <v>0.18042195912175801</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="10">
+      <c r="A14" s="7">
         <v>1</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="10">
+      <c r="A15" s="7">
         <v>2</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2445,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4499C35-C495-40C1-9CBB-51EA8FFA5990}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2456,196 +2323,195 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="26"/>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="24" t="s">
+      <c r="C1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="20"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="11">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="18">
+      <c r="D2" s="11">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
         <v>2</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="11">
         <f>POWER(B2,2)/(B6*$E2)</f>
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="11">
         <f>POWER(C2,2)/(C6*$E2)</f>
         <v>0.2</v>
       </c>
-      <c r="I2" s="18">
+      <c r="I2" s="11">
         <f>POWER(D2,2)/(D6*$E2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="11">
         <v>8</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="11">
         <v>4</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="11">
         <v>13</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="11">
         <f>POWER(B3,2)/(B$6*$E3)</f>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="11">
         <f>POWER(C3,2)/(C$6*$E3)</f>
         <v>0.49230769230769234</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="11">
         <f>POWER(D3,2)/(D$6*$E3)</f>
         <v>0.24615384615384617</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="18">
-        <v>0</v>
-      </c>
-      <c r="G4" s="19">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1">
-      <c r="A5" s="19" t="s">
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
         <v>1</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="11">
         <v>1</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="11">
         <f>POWER(B5,2)/(B$6*$E5)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="11">
         <f>POWER(C5,2)/(C$6*$E5)</f>
         <v>0</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="11">
         <f>POWER(D5,2)/(D$6*$E5)</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:9">
+      <c r="A6" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="11">
         <v>10</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="11">
         <v>5</v>
       </c>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1"/>
-    <row r="9" spans="1:9" ht="15" thickBot="1">
-      <c r="A9" s="14" t="s">
+      <c r="E6" s="11"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <f>SUM(G2:I5)-1</f>
         <v>0.21538461538461529</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="s">
         <v>90</v>
       </c>
       <c r="E9" s="12">
-        <f>B9/((4-1)*(3-1))</f>
-        <v>3.5897435897435881E-2</v>
+        <f>SQRT(B9/((4-1)*(3-1)))</f>
+        <v>0.18946618668626833</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="10">
+      <c r="A13" s="7">
         <v>1</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="10">
+      <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2659,10 +2525,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6594F93-0BF1-482F-ADDA-2E43BB81A600}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2670,159 +2536,195 @@
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="26"/>
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="20"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="19" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="11"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="11">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="11">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="11">
         <v>3</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="11">
         <v>8</v>
       </c>
-      <c r="G2" s="19">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11">
         <f>POWER(B2,2)/(B4*$E2)</f>
         <v>0.125</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="11">
         <f>POWER(C2,2)/(C4*$E2)</f>
         <v>0.1875</v>
       </c>
-      <c r="I2" s="18">
+      <c r="I2" s="11">
         <f>POWER(D2,2)/(D4*$E2)</f>
         <v>0.1875</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1">
-      <c r="A3" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="11">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="11">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="11">
         <v>3</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="11">
         <v>8</v>
       </c>
-      <c r="G3" s="17">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11">
         <f>POWER(B3,2)/(B$4*$E3)</f>
         <v>0.125</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="11">
         <f>POWER(C3,2)/(C$4*$E3)</f>
         <v>0.1875</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="11">
         <f>POWER(D3,2)/(D$4*$E3)</f>
         <v>0.1875</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1">
-      <c r="A4" s="17" t="s">
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="11">
         <v>4</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="11">
         <v>6</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="11">
         <v>6</v>
       </c>
-      <c r="E4" s="15"/>
-    </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1"/>
-    <row r="7" spans="1:15" ht="15" thickBot="1">
-      <c r="A7" s="14" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <f>SUM(G2:I3)-1</f>
         <v>0</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
         <v>90</v>
       </c>
       <c r="E7" s="12">
-        <f>B7/((2-1)*(3-1))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="O9" s="11"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="10">
+        <f>SQRT(B7/((2-1)*(3-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="7">
         <v>1</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="10">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="7">
         <v>2</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>